<commit_message>
Updated spreadsheet in test fixtures
</commit_message>
<xml_diff>
--- a/tests/fixtures/log.xlsx
+++ b/tests/fixtures/log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7763C0C9-AC78-2842-9208-29E173B08D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E0775F9-A8BF-9A45-8CF7-94E5E136A1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="2160" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,33 +20,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+  <si>
+    <t>Recipe</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>YYYY</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
   <si>
     <t>Label</t>
   </si>
   <si>
-    <t>File</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>YYYY</t>
-  </si>
-  <si>
-    <t>MM</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
     <t>Example</t>
   </si>
   <si>
     <t>tests/fixtures/source/DOE^JOHN-002304/20200312-scan1.dcm</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
   <si>
     <t>DOE^JOHN</t>
@@ -458,16 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="8.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,163 +499,187 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="G3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
       </c>
       <c r="H3" t="s">
         <v>16</v>
       </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="H4" t="s">
-        <v>14</v>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload tests now passing
</commit_message>
<xml_diff>
--- a/tests/fixtures/log.xlsx
+++ b/tests/fixtures/log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F86BEE-9F4B-D445-93FC-1B8CD23EA528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAB1280-AB50-7A4E-A81B-D039A47FB683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="11620" windowWidth="14400" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>